<commit_message>
Android Game 2048 learning 1
</commit_message>
<xml_diff>
--- a/応用情報午前試験統計.xlsx
+++ b/応用情報午前試験統計.xlsx
@@ -54,6 +54,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,14 +106,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,7 +419,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -426,29 +429,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
       <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,74 +579,125 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
-        <v>42705</v>
-      </c>
-      <c r="D4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O4" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q4" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="A4" s="3">
+        <v>42709.40347222222</v>
+      </c>
+      <c r="B4">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>64</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>59.4</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>66.7</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="7"/>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="D5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K5" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O5" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q5" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="A5" s="2">
+        <v>42709.585416666669</v>
+      </c>
+      <c r="B5">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>56</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>73.2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>83.3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>18</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>55.6</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="7"/>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">

</xml_diff>